<commit_message>
Added expert values to tcp_params.xlsx
</commit_message>
<xml_diff>
--- a/tcp_params.xlsx
+++ b/tcp_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="165">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -230,9 +230,6 @@
     <t>tcp_fastopen</t>
   </si>
   <si>
-    <t>Could boost short-lived flows.</t>
-  </si>
-  <si>
     <t>tcp_timestamps</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>tcp_tw_reuse</t>
   </si>
   <si>
-    <t>Nothing to do with performance</t>
-  </si>
-  <si>
     <t>tcp_window_scaling</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Chosen Range</t>
-  </si>
-  <si>
     <t>Irrelevant. Kernel periodically reprobes path for changed MTU anyway. This value is only for the beginning.</t>
   </si>
   <si>
@@ -335,9 +326,6 @@
     <t>Consider the most forward selective acknowledgement sequence number as a sign that all the previous un-(selectively)-acknowledged segments were lost.</t>
   </si>
   <si>
-    <t>Widely used value</t>
-  </si>
-  <si>
     <t>How long to keep socket in FIN_WAIT_2.</t>
   </si>
   <si>
@@ -413,9 +401,6 @@
     <t>Turning this on can supposedly degrqde performance, since the kernel has to store some additional state for each connection. Carrying out tests, I didn't notice any difference in performance!</t>
   </si>
   <si>
-    <t>influences the timeout of a locally closed TCP connection, when RTO retransmissions remain unacknowledged.</t>
-  </si>
-  <si>
     <t>0 - no orphans</t>
   </si>
   <si>
@@ -489,6 +474,51 @@
   </si>
   <si>
     <t>Limited by tcp_mem</t>
+  </si>
+  <si>
+    <t>"Expert" value</t>
+  </si>
+  <si>
+    <t>Plotted</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4096, 87380, 16777216) [1 GE] </t>
+  </si>
+  <si>
+    <t>depends on app</t>
+  </si>
+  <si>
+    <t>&gt; 128k</t>
+  </si>
+  <si>
+    <t>Leave it alone</t>
+  </si>
+  <si>
+    <t>9 to 15</t>
+  </si>
+  <si>
+    <t>Only to prevent DDoS. Each orphan can eat up to max_wmem unswappable memory.</t>
+  </si>
+  <si>
+    <t>2 to 5</t>
+  </si>
+  <si>
+    <t>Could boost short-lived flows. Some Firewalls do not like it.</t>
+  </si>
+  <si>
+    <t>(8192, 65536, 16777216)</t>
+  </si>
+  <si>
+    <t>Recycle can break clients behind NAT.</t>
+  </si>
+  <si>
+    <t>Try to re-use TIME-WAIT connections.</t>
+  </si>
+  <si>
+    <t>Influences the timeout of a locally closed TCP connection, when RTO retransmissions remain unacknowledged.</t>
   </si>
 </sst>
 </file>
@@ -549,7 +579,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -572,11 +602,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -620,6 +661,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,8 +1029,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,48 +1039,48 @@
     <col min="2" max="2" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1041,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1049,18 +1096,24 @@
       <c r="D2" s="8">
         <v>0</v>
       </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="2" t="s">
-        <v>81</v>
+      <c r="I2" s="10"/>
+      <c r="J2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -1068,7 +1121,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1076,20 +1129,26 @@
       <c r="D3" s="8">
         <v>1</v>
       </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G3" s="9" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>84</v>
+      <c r="J3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1097,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1105,16 +1164,19 @@
       <c r="D4" s="8">
         <v>31</v>
       </c>
+      <c r="E4" s="8">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1123,26 +1185,29 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1150,7 +1215,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1158,18 +1223,24 @@
       <c r="D6" s="8">
         <v>512</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="E6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="2" t="s">
-        <v>91</v>
+      <c r="I6" s="10"/>
+      <c r="J6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1177,25 +1248,28 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1204,7 +1278,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1212,20 +1286,26 @@
       <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>96</v>
+        <v>15</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1233,31 +1313,34 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="9" t="s">
         <v>87</v>
       </c>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="H9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J9" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1265,18 +1348,21 @@
       <c r="D10" s="8">
         <v>2</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>3</v>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1284,26 +1370,29 @@
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>3</v>
+        <v>87</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="64" x14ac:dyDescent="0.2">
@@ -1311,7 +1400,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1319,17 +1408,23 @@
       <c r="D12" s="8">
         <v>1</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>94</v>
+        <v>15</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1337,7 +1432,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1345,23 +1440,26 @@
       <c r="D13" s="8">
         <v>60</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="E13" s="8">
+        <v>30</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1369,16 +1467,19 @@
       <c r="D14" s="8">
         <v>2</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="2" t="s">
-        <v>106</v>
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1386,56 +1487,56 @@
         <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>87</v>
+        <v>106</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>3</v>
+        <v>105</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1443,7 +1544,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1451,26 +1552,26 @@
       <c r="D17" s="8">
         <v>9</v>
       </c>
-      <c r="E17" s="8">
-        <v>9</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>3</v>
+      <c r="E17" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1478,17 +1579,20 @@
       <c r="D18" s="8">
         <v>75</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>3</v>
+      <c r="E18" s="8">
+        <v>30</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1497,7 +1601,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1505,23 +1609,26 @@
       <c r="D19" s="8">
         <v>0</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>3</v>
+      <c r="E19" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J19" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1529,18 +1636,21 @@
       <c r="D20" s="8">
         <v>262144</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>3</v>
+      <c r="E20" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="2" t="s">
-        <v>33</v>
+        <v>85</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1548,7 +1658,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1556,17 +1666,20 @@
       <c r="D21" s="8">
         <v>2048</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>3</v>
+      <c r="E21" s="8">
+        <v>8096</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1575,7 +1688,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1583,17 +1696,20 @@
       <c r="D22" s="8">
         <v>262144</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>3</v>
+      <c r="E22" s="8">
+        <v>1440000</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1602,27 +1718,30 @@
         <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="K23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1631,34 +1750,34 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="8">
         <v>300</v>
       </c>
+      <c r="F24" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G24" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J24" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1666,13 +1785,16 @@
       <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="2" t="s">
+      <c r="I25" s="10"/>
+      <c r="J25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1681,7 +1803,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -1689,17 +1811,20 @@
       <c r="D26" s="8">
         <v>0</v>
       </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="15" t="s">
+      <c r="I26" s="10"/>
+      <c r="J26" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1708,16 +1833,19 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>15</v>
@@ -1725,11 +1853,8 @@
       <c r="H27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="15" t="s">
+      <c r="I27" s="10"/>
+      <c r="J27" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1738,13 +1863,19 @@
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>15</v>
@@ -1752,11 +1883,8 @@
       <c r="H28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="15" t="s">
+      <c r="I28" s="10"/>
+      <c r="J28" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1765,7 +1893,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1776,18 +1904,21 @@
       <c r="E29" s="8">
         <v>1</v>
       </c>
+      <c r="F29" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G29" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="2" t="s">
-        <v>128</v>
+        <v>85</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1795,26 +1926,29 @@
         <v>48</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="2" t="s">
-        <v>131</v>
+        <v>85</v>
+      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1822,25 +1956,28 @@
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="J31" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1849,22 +1986,25 @@
         <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
+      <c r="E32" s="8">
+        <v>3</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G32" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1873,28 +2013,28 @@
         <v>53</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E33" s="8">
         <v>300</v>
       </c>
+      <c r="F33" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G33" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I33" s="10"/>
+      <c r="J33" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1903,31 +2043,28 @@
         <v>54</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="10"/>
+      <c r="J34" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1936,7 +2073,7 @@
         <v>56</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1947,23 +2084,26 @@
       <c r="E35" s="8">
         <v>3</v>
       </c>
+      <c r="F35" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G35" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J35" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="I35" s="10"/>
+      <c r="K35" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1974,29 +2114,38 @@
       <c r="E36" s="8">
         <v>15</v>
       </c>
+      <c r="F36" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G36" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="I36" s="10"/>
+      <c r="K36" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>15</v>
@@ -2004,13 +2153,10 @@
       <c r="H37" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="K37" s="2" t="s">
+      <c r="I37" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2019,7 +2165,7 @@
         <v>60</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -2027,18 +2173,24 @@
       <c r="D38" s="8">
         <v>1</v>
       </c>
+      <c r="E38" s="8">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G38" s="9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J38" s="10"/>
-      <c r="K38" s="2" t="s">
-        <v>141</v>
+        <v>15</v>
+      </c>
+      <c r="I38" s="10"/>
+      <c r="J38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2046,7 +2198,7 @@
         <v>61</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -2054,17 +2206,17 @@
       <c r="D39" s="8">
         <v>0</v>
       </c>
+      <c r="F39" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G39" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J39" s="10"/>
-      <c r="K39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" s="10"/>
+      <c r="J39" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2073,7 +2225,7 @@
         <v>62</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -2081,20 +2233,20 @@
       <c r="D40" s="8">
         <v>5</v>
       </c>
-      <c r="E40" s="8">
-        <v>5</v>
+      <c r="E40" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="10"/>
-      <c r="K40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="10"/>
+      <c r="J40" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2103,7 +2255,7 @@
         <v>63</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -2114,17 +2266,17 @@
       <c r="E41" s="8">
         <v>5</v>
       </c>
+      <c r="F41" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G41" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J41" s="10"/>
-      <c r="K41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="10"/>
+      <c r="J41" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2133,7 +2285,7 @@
         <v>64</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -2141,14 +2293,20 @@
       <c r="D42" s="8">
         <v>1</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="E42" s="8">
+        <v>1</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="9"/>
       <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="2" t="s">
+      <c r="I42" s="10"/>
+      <c r="J42" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2156,58 +2314,67 @@
         <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="E43" s="8">
+        <v>3</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J43" s="10"/>
-      <c r="K43" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
+      </c>
+      <c r="I43" s="10"/>
+      <c r="J43" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
         <v>21</v>
       </c>
+      <c r="E44" s="8">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G44" s="9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J44" s="10"/>
-      <c r="K44" s="2" t="s">
-        <v>149</v>
+        <v>15</v>
+      </c>
+      <c r="I44" s="10"/>
+      <c r="J44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -2215,26 +2382,29 @@
       <c r="D45" s="8">
         <v>0</v>
       </c>
+      <c r="E45" s="8">
+        <v>0</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G45" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J45" s="10"/>
-      <c r="K45" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -2242,26 +2412,29 @@
       <c r="D46" s="8">
         <v>0</v>
       </c>
+      <c r="E46" s="8">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G46" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J46" s="10"/>
-      <c r="K46" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -2272,32 +2445,38 @@
       <c r="E47" s="8">
         <v>1</v>
       </c>
+      <c r="F47" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G47" s="9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="10"/>
-      <c r="K47" s="2" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="I47" s="10"/>
+      <c r="J47" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C48" t="s">
         <v>40</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>15</v>
@@ -2305,18 +2484,18 @@
       <c r="H48" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="K48" s="2" t="s">
+      <c r="I48" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="K48" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -2324,7 +2503,7 @@
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:J1048576">
+  <conditionalFormatting sqref="F1:I1048576 K1 K38">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -2332,7 +2511,7 @@
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -2340,7 +2519,7 @@
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
+  <conditionalFormatting sqref="H48">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -2349,5 +2528,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated params file. From now on moving to Google Docs
</commit_message>
<xml_diff>
--- a/tcp_params.xlsx
+++ b/tcp_params.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$K</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="165">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -194,12 +197,6 @@
     <t>Irrelevant</t>
   </si>
   <si>
-    <t>tcp_retries_1</t>
-  </si>
-  <si>
-    <t>tcp_retries_2</t>
-  </si>
-  <si>
     <t>tcp_rmem</t>
   </si>
   <si>
@@ -519,13 +516,19 @@
   </si>
   <si>
     <t>Influences the timeout of a locally closed TCP connection, when RTO retransmissions remain unacknowledged.</t>
+  </si>
+  <si>
+    <t>tcp_retries1</t>
+  </si>
+  <si>
+    <t>tcp_retries2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -548,6 +551,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -617,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -666,6 +675,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1030,7 +1042,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,7 +1051,7 @@
     <col min="2" max="2" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16" style="8" customWidth="1"/>
     <col min="6" max="6" width="8" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="8" bestFit="1" customWidth="1"/>
@@ -1053,34 +1065,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1088,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1110,10 +1122,10 @@
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -1121,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1133,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>3</v>
@@ -1145,10 +1157,10 @@
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1156,7 +1168,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1168,7 +1180,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>3</v>
@@ -1178,6 +1190,9 @@
       </c>
       <c r="I4" s="10" t="s">
         <v>4</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1185,29 +1200,32 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1215,7 +1233,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1224,7 +1242,7 @@
         <v>512</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>3</v>
@@ -1237,10 +1255,10 @@
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1248,16 +1266,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>15</v>
@@ -1266,19 +1284,22 @@
         <v>3</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="K7" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1299,13 +1320,13 @@
         <v>15</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="K8" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1313,34 +1334,37 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="8">
         <v>2</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I9" s="12"/>
+      <c r="K9" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1355,14 +1379,17 @@
         <v>3</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1370,29 +1397,32 @@
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="64" x14ac:dyDescent="0.2">
@@ -1400,7 +1430,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1421,10 +1451,10 @@
         <v>15</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1432,7 +1462,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1453,13 +1483,16 @@
         <v>3</v>
       </c>
       <c r="I13" s="10"/>
+      <c r="K13" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1479,7 +1512,10 @@
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1487,56 +1523,62 @@
         <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="10"/>
+      <c r="K15" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1544,7 +1586,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1553,25 +1595,28 @@
         <v>9</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I17" s="10"/>
+      <c r="K17" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1586,22 +1631,25 @@
         <v>3</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="K18" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1610,25 +1658,28 @@
         <v>0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I19" s="10"/>
+      <c r="K19" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1637,20 +1688,23 @@
         <v>262144</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1658,7 +1712,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1673,22 +1727,25 @@
         <v>3</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="K21" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1703,31 +1760,34 @@
         <v>3</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="K22" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>15</v>
@@ -1739,10 +1799,13 @@
         <v>15</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1750,34 +1813,37 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="8">
         <v>300</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I24" s="10"/>
+      <c r="K24" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1797,13 +1863,16 @@
       <c r="J25" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="K25" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -1827,22 +1896,25 @@
       <c r="J26" s="15" t="s">
         <v>44</v>
       </c>
+      <c r="K26" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>15</v>
@@ -1857,22 +1929,25 @@
       <c r="J27" s="15" t="s">
         <v>44</v>
       </c>
+      <c r="K27" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>15</v>
@@ -1887,13 +1962,16 @@
       <c r="J28" s="15" t="s">
         <v>44</v>
       </c>
+      <c r="K28" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1908,17 +1986,17 @@
         <v>3</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1926,13 +2004,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E30" s="8">
         <v>0</v>
@@ -1941,14 +2019,17 @@
         <v>3</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1956,37 +2037,40 @@
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="K31" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1995,85 +2079,94 @@
         <v>3</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="K32" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E33" s="8">
         <v>300</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="K33" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="K34" s="18" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -2085,25 +2178,25 @@
         <v>3</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I35" s="10"/>
       <c r="K35" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -2115,34 +2208,34 @@
         <v>15</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I36" s="10"/>
       <c r="K36" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>15</v>
@@ -2154,18 +2247,21 @@
         <v>15</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -2187,18 +2283,18 @@
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -2210,22 +2306,25 @@
         <v>3</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="K39" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -2234,28 +2333,31 @@
         <v>5</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>3</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -2270,22 +2372,25 @@
         <v>3</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>3</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -2303,48 +2408,51 @@
       <c r="H42" s="9"/>
       <c r="I42" s="10"/>
       <c r="J42" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" s="8">
         <v>3</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
         <v>21</v>
@@ -2363,18 +2471,18 @@
       </c>
       <c r="I44" s="10"/>
       <c r="J44" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -2389,22 +2497,25 @@
         <v>3</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -2419,22 +2530,25 @@
         <v>3</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -2456,24 +2570,27 @@
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
         <v>40</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>15</v>
@@ -2485,16 +2602,17 @@
         <v>15</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"NO"</formula>
@@ -2527,7 +2645,7 @@
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>